<commit_message>
Pushing simulator byte format doc to server.
</commit_message>
<xml_diff>
--- a/Documents/SimulatorByteFormatIntegration.xlsx
+++ b/Documents/SimulatorByteFormatIntegration.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="308">
   <si>
     <t>[0]</t>
   </si>
@@ -938,6 +938,9 @@
   </si>
   <si>
     <t>This is an example of the message values and structure of data streamed out of xplane when the 'internet via UDP' checkbox is checked for message ID's 8, 16, 17, 20, 21, 39, in the data input &amp; output screen of X-Plane 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G223"/>
+  <dimension ref="A1:H223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1340,7 @@
     <col min="8" max="16384" width="28.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>306</v>
       </c>
@@ -1347,8 +1350,11 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>295</v>
       </c>
@@ -1371,7 +1377,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>301</v>
       </c>
@@ -1385,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>302</v>
       </c>
@@ -1399,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>303</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>304</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>305</v>
       </c>
@@ -1441,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>290</v>
       </c>
@@ -1455,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1466,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1477,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1488,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>80</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>80</v>
       </c>
@@ -1534,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>80</v>
       </c>
@@ -1557,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>80</v>
       </c>
@@ -1580,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>82</v>
       </c>

</xml_diff>